<commit_message>
upload final version for Thur Oct 4th meeting
</commit_message>
<xml_diff>
--- a/Reports/soi_analysis.xlsx
+++ b/Reports/soi_analysis.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-3030" yWindow="2655" windowWidth="20730" windowHeight="7455" activeTab="2"/>
+    <workbookView xWindow="580" yWindow="60" windowWidth="15740" windowHeight="11980" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AGN" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="AMZN" sheetId="3" r:id="rId3"/>
+    <sheet name="BA" sheetId="4" r:id="rId4"/>
+    <sheet name="CAT" sheetId="5" r:id="rId5"/>
+    <sheet name="TIF" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="132">
   <si>
     <t>Avg Delay</t>
   </si>
@@ -214,24 +222,266 @@
   </si>
   <si>
     <t>Key (delay(s)_decay)</t>
+  </si>
+  <si>
+    <t>0.01_1.25</t>
+  </si>
+  <si>
+    <t>0.025_0.5</t>
+  </si>
+  <si>
+    <t>0.01_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.01_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.02_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_1.25</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.005_0.75</t>
+  </si>
+  <si>
+    <t>0_0.005_1</t>
+  </si>
+  <si>
+    <t>0.02_0.75</t>
+  </si>
+  <si>
+    <t>005_0.75</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.005_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.015_0.75</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.01_0.75</t>
+  </si>
+  <si>
+    <t>0.005_0.75</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.095_0.75</t>
+  </si>
+  <si>
+    <t>0_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.04_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.07_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.005_1.25</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.04_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.01_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.015_0.5</t>
+  </si>
+  <si>
+    <t>Key</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.045_0.75</t>
+  </si>
+  <si>
+    <t>0.09_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.05_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.095_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.025_1.25</t>
+  </si>
+  <si>
+    <t>0.055_1.5</t>
+  </si>
+  <si>
+    <t>0.05_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.03_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.045_1.5</t>
+  </si>
+  <si>
+    <t>0.05_1.25</t>
+  </si>
+  <si>
+    <t>00_0.05_1</t>
+  </si>
+  <si>
+    <t>0.03_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_0.75</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_0.04_1</t>
+  </si>
+  <si>
+    <t>0_0.03_1</t>
+  </si>
+  <si>
+    <t>0.065_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.045_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.035_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.015_1.5</t>
+  </si>
+  <si>
+    <t>.015_1.25</t>
+  </si>
+  <si>
+    <t>0.02_1.25</t>
+  </si>
+  <si>
+    <t>0.02_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.02_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.06_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.075_1.5</t>
+  </si>
+  <si>
+    <t>.075_1.25</t>
+  </si>
+  <si>
+    <t>0.08_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.07_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.095_1.25</t>
+  </si>
+  <si>
+    <t>0.1_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.09_1.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1_1.25</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.055_1.25</t>
+  </si>
+  <si>
+    <t>.085_1.25</t>
+  </si>
+  <si>
+    <t>0.08_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>.095_0.5</t>
+  </si>
+  <si>
+    <t>0_0.75</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0_1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -239,7 +489,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -247,7 +497,29 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -270,26 +542,26 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -298,7 +570,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -306,17 +578,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -326,7 +598,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -334,12 +606,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -348,27 +620,27 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -376,27 +648,27 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -404,32 +676,176 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -447,15 +863,6 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -479,15 +886,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -509,10 +907,190 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+  <cellStyles count="146">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="144" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -814,25 +1392,25 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1">
       <c r="A1" s="14">
         <v>41387</v>
       </c>
@@ -855,51 +1433,51 @@
       </c>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:11" ht="15" thickBot="1">
+      <c r="A2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="17" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="22"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="19"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="18" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="15"/>
-      <c r="G3" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="20" t="s">
+      <c r="G3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="20" t="s">
+      <c r="I3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -932,7 +1510,7 @@
         <v>0.43066070233138998</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -965,7 +1543,7 @@
         <v>0.42200730834584699</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -998,7 +1576,7 @@
         <v>0.41995811554669799</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1031,7 +1609,7 @@
         <v>0.41771746131776599</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1064,51 +1642,51 @@
         <v>0.41741298145731598</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:11" ht="15" thickBot="1">
+      <c r="A9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="17" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="22"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="39"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickBot="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="19"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="18" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="15"/>
-      <c r="G10" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="20" t="s">
+      <c r="G10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="20" t="s">
+      <c r="I10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -1141,7 +1719,7 @@
         <v>1.30303420370288E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
@@ -1174,7 +1752,7 @@
         <v>8.0483518362288696E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1207,7 +1785,7 @@
         <v>5.0602616580138803E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1818,7 @@
         <v>4.4855283745562904E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
@@ -1273,7 +1851,7 @@
         <v>2.4354227114006298E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1282,7 +1860,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15" thickBot="1">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1291,41 +1869,41 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="43" thickBot="1">
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" thickBot="1">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="20">
         <v>0.35539929999999997</v>
       </c>
       <c r="C20" s="9">
         <v>0.43066070233138998</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="21">
         <v>0</v>
       </c>
       <c r="E20" s="11">
         <v>1.30303420370288E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1344,7 +1922,14 @@
     <mergeCell ref="H9:K9"/>
     <mergeCell ref="H2:K2"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1353,34 +1938,34 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:4" ht="29" thickBot="1">
+      <c r="A1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>38</v>
       </c>
@@ -1394,26 +1979,26 @@
         <v>0.43066070233138998</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:4" ht="29" thickBot="1">
+      <c r="A3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" thickBot="1">
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="21">
         <v>0</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="11">
@@ -1421,7 +2006,13 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1429,126 +2020,126 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32">
+    <row r="1" spans="1:10" ht="15" thickBot="1">
+      <c r="A1" s="26">
         <v>41387</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34">
+      <c r="B1" s="27"/>
+      <c r="C1" s="28">
         <v>41388</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34">
+      <c r="D1" s="27"/>
+      <c r="E1" s="28">
         <v>41389</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="32">
+      <c r="F1" s="29"/>
+      <c r="G1" s="26">
         <v>41390</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34">
+      <c r="H1" s="27"/>
+      <c r="I1" s="28">
         <v>41393</v>
       </c>
-      <c r="J1" s="35"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="J1" s="29"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="A2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="29" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1">
+      <c r="A3" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="37" t="s">
+      <c r="B3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="36" t="s">
+      <c r="F3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="36" t="s">
+      <c r="H3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B4" s="36">
         <v>0.29910863735427701</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="35">
         <v>6.4969415225430496E-2</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="36">
         <v>4.2028309925023703E-2</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="36">
         <v>0.20731118345604199</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="36">
         <v>0.16668124597032699</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
@@ -1580,7 +2171,7 @@
         <v>0.164777656593185</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
@@ -1612,7 +2203,7 @@
         <v>0.163919121731016</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="4" t="s">
         <v>44</v>
       </c>
@@ -1644,7 +2235,7 @@
         <v>0.158924224073314</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1">
       <c r="A8" s="8" t="s">
         <v>45</v>
       </c>
@@ -1676,87 +2267,87 @@
         <v>0.15621657225833499</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="A9" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="29" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="31"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39" t="s">
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1">
+      <c r="A10" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="40" t="s">
+      <c r="B10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="39" t="s">
+      <c r="D10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="36" t="s">
+      <c r="F10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="36" t="s">
+      <c r="H10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="36">
         <v>0.19342766090074201</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="35">
         <v>4.4907265119989798E-2</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="36">
         <v>8.2163688079832306E-2</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="42">
+      <c r="H11" s="36">
         <v>9.0721235288243093E-2</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="36">
         <v>0.19538943177224799</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
@@ -1788,7 +2379,7 @@
         <v>0.193503440482683</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
@@ -1820,7 +2411,7 @@
         <v>0.18692134417184</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
@@ -1852,7 +2443,7 @@
         <v>0.184200059853703</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1">
       <c r="A15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1891,6 +2482,1762 @@
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="G9:J9"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1">
+      <c r="A1" s="49">
+        <v>41387</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49">
+        <v>41388</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49">
+        <v>41389</v>
+      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49">
+        <v>41390</v>
+      </c>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49">
+        <v>41393</v>
+      </c>
+      <c r="J1" s="48"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="A2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1">
+      <c r="A3" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="45">
+        <v>8.1337687618641102E-2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="45">
+        <v>0.106422435719598</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="45">
+        <v>8.4712149400242395E-2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="45">
+        <v>3.91385283935861E-2</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J4" s="45">
+        <v>8.7259274914507204E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="46">
+        <v>8.0853436772845497E-2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="46">
+        <v>0.103227588286876</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="46">
+        <v>4.6070405526546697E-2</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="46">
+        <v>3.8493360019465198E-2</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="46">
+        <v>8.0185046299375604E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="46">
+        <v>7.8216213962069597E-2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="46">
+        <v>8.7236841134644402E-2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="46">
+        <v>4.4881573715758301E-2</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="46">
+        <v>3.7983324006073002E-2</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="46">
+        <v>7.8163537961277799E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="46">
+        <v>7.5439341062293705E-2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="46">
+        <v>8.5980014132261404E-2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="46">
+        <v>4.4435357731152599E-2</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="46">
+        <v>3.5096799347339801E-2</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="46">
+        <v>7.2244167176393301E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="47">
+        <v>7.4890981870377002E-2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="47">
+        <v>8.4863093288677E-2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="47">
+        <v>4.4383205933338998E-2</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" s="47">
+        <v>3.49431642636331E-2</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="47">
+        <v>7.1640988664793404E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="A9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1">
+      <c r="A10" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="45">
+        <v>5.7539249215492402E-2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="45">
+        <v>0.134033492176235</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="45">
+        <v>0.103363678617353</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="45">
+        <v>2.03371648759825E-2</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="45">
+        <v>9.27668878335981E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="46">
+        <v>4.8540942723489702E-2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="46">
+        <v>0.131220416913855</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="46">
+        <v>6.6177689615593102E-2</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="46">
+        <v>1.9979984054138901E-2</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="46">
+        <v>9.0853900733310303E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="46">
+        <v>4.8475877306385598E-2</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="46">
+        <v>0.12976732179532199</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="46">
+        <v>6.5078325581315793E-2</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="46">
+        <v>1.8831944312150701E-2</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="46">
+        <v>8.6926023775470707E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="46">
+        <v>4.5570550113140498E-2</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="46">
+        <v>0.12812745102005799</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="46">
+        <v>6.4407837619424396E-2</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="46">
+        <v>1.87177650985191E-2</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="46">
+        <v>7.0578540686354302E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="47">
+        <v>4.49808010193102E-2</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="47">
+        <v>0.12677120721092899</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="47">
+        <v>6.2526932213518197E-2</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="47">
+        <v>1.51522593541618E-2</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J15" s="47">
+        <v>6.9269750162156196E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="str">
+        <f>RIGHT(A4,9)</f>
+        <v>0.005_0.5</v>
+      </c>
+      <c r="C17" t="str">
+        <f>RIGHT(C11,9)</f>
+        <v>0.02_0.75</v>
+      </c>
+      <c r="E17" t="str">
+        <f>RIGHT(E4,9)</f>
+        <v>0_0.5</v>
+      </c>
+      <c r="G17" t="str">
+        <f>RIGHT(G4,9)</f>
+        <v>0.04_0.5</v>
+      </c>
+      <c r="I17" t="str">
+        <f>RIGHT(I4,9)</f>
+        <v>0.01_0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="str">
+        <f t="shared" ref="A18:A21" si="0">RIGHT(A5,9)</f>
+        <v>0.01_1.5</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" ref="C18:E21" si="1">RIGHT(C12,9)</f>
+        <v>0.02_0.5</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" ref="E18:E21" si="2">RIGHT(E5,9)</f>
+        <v>0.005_0.5</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" ref="G18:G21" si="3">RIGHT(G5,9)</f>
+        <v>0.04_0.75</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" ref="I18:I21" si="4">RIGHT(I5,9)</f>
+        <v>0.015_0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>0.01_1.25</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>0.01_0.75</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>.005_0.75</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
+        <v>0.01_0.75</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="4"/>
+        <v>0.005_0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>0.025_0.5</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>0.03_0.75</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>0.005_1.5</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
+        <v>0.01_1</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="4"/>
+        <v>0.025_0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>0.01_1</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>.005_0.75</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>0.005_1</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
+        <v>0.01_0.5</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="4"/>
+        <v>0.01_0.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1">
+      <c r="A1" s="49">
+        <v>41387</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49">
+        <v>41388</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49">
+        <v>41389</v>
+      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49">
+        <v>41390</v>
+      </c>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49">
+        <v>41393</v>
+      </c>
+      <c r="J1" s="48"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="A2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1">
+      <c r="A3" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="46">
+        <v>0.10198103837449</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="45">
+        <v>0.13024883995761599</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="45">
+        <v>0.13731800041480999</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="45">
+        <v>0.108409126053283</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="45">
+        <v>7.9119580441904702E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="46">
+        <v>9.4820049168795703E-2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="46">
+        <v>0.13012249962521899</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="46">
+        <v>0.13108931299553001</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="46">
+        <v>0.10681504834807699</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="46">
+        <v>7.7731544583786796E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="46">
+        <v>9.1430131953623206E-2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="46">
+        <v>0.13007448341026101</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="46">
+        <v>0.126121046223926</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="46">
+        <v>9.5624523397768696E-2</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="46">
+        <v>7.7567588161967599E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="46">
+        <v>8.9763748524438094E-2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0.12899199474737</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="46">
+        <v>0.124211355164473</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="46">
+        <v>9.3123310563318795E-2</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="46">
+        <v>7.6958456227868302E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1">
+      <c r="A8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="46">
+        <v>8.6229436248692795E-2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="47">
+        <v>6.1357358932683501E-2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="47">
+        <v>0.12377494701285099</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="47">
+        <v>8.6556505507740203E-2</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="47">
+        <v>7.6711097025810401E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="A9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1">
+      <c r="A10" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="45">
+        <v>0.73127040666218801</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="45">
+        <v>7.1316565212162106E-2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="45">
+        <v>0.32592379761686002</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H11" s="45">
+        <v>6.4268568320558606E-2</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="45">
+        <v>7.5300530326204901E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="46">
+        <v>0.62538558427318103</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="46">
+        <v>6.2096510098843601E-2</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="46">
+        <v>0.31525395849071802</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="46">
+        <v>6.4109155837396695E-2</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="46">
+        <v>7.2689028567358302E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="46">
+        <v>0.54980267412248696</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="46">
+        <v>5.5731834091713298E-2</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="46">
+        <v>0.31488319050945701</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="46">
+        <v>5.3290006450426697E-2</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="46">
+        <v>7.0241016908925397E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="46">
+        <v>0.42579709940218502</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="46">
+        <v>5.5531242334657997E-2</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="46">
+        <v>0.31033786067552199</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="46">
+        <v>5.1854446493115901E-2</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="46">
+        <v>6.98165588905445E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1">
+      <c r="A15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="47">
+        <v>0.36074409635714599</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="47">
+        <v>5.5108504176604498E-2</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="47">
+        <v>0.30545669887341897</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="47">
+        <v>4.9954453170906001E-2</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="47">
+        <v>6.7807204486495604E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="str">
+        <f>RIGHT(A11,9)</f>
+        <v>0_0.5</v>
+      </c>
+      <c r="C17" t="str">
+        <f>RIGHT(C11,9)</f>
+        <v>0.01_0.5</v>
+      </c>
+      <c r="E17" t="str">
+        <f>RIGHT(E4,9)</f>
+        <v>0.025_1.5</v>
+      </c>
+      <c r="G17" t="str">
+        <f>RIGHT(G4,9)</f>
+        <v>0.095_0.5</v>
+      </c>
+      <c r="I17" t="str">
+        <f>RIGHT(I4,9)</f>
+        <v>0.04_0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="str">
+        <f t="shared" ref="A18" si="0">RIGHT(A12,9)</f>
+        <v>0_0.75</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" ref="A18:C22" si="1">RIGHT(C12,9)</f>
+        <v>0.01_0.75</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" ref="E18:E21" si="2">RIGHT(E5,9)</f>
+        <v>0.05_1.5</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" ref="G18:G21" si="3">RIGHT(G5,9)</f>
+        <v>0.09_0.5</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" ref="I18:I21" si="4">RIGHT(I5,9)</f>
+        <v>0.045_0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="str">
+        <f t="shared" ref="A19" si="5">RIGHT(A13,9)</f>
+        <v>0_1</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>0.03_0.75</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>0.045_1.5</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
+        <v>.095_0.75</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="4"/>
+        <v>0.04_0.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="str">
+        <f t="shared" ref="A20" si="6">RIGHT(A14,9)</f>
+        <v>0_1.25</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>0.03_0.5</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>.025_1.25</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
+        <v>0.09_0.75</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="4"/>
+        <v>0.055_0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="str">
+        <f t="shared" ref="A21" si="7">RIGHT(A15,9)</f>
+        <v>0.01_0.5</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>0.01_1</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>0.055_1.5</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
+        <v>0.095_1</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="4"/>
+        <v>.045_0.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:J2"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1">
+      <c r="A1" s="49">
+        <v>41387</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49">
+        <v>41388</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="49">
+        <v>41389</v>
+      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49">
+        <v>41390</v>
+      </c>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49">
+        <v>41393</v>
+      </c>
+      <c r="J1" s="48"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1">
+      <c r="A2" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1">
+      <c r="A3" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="46">
+        <v>8.1055813526583198E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="46">
+        <v>0.20988579643590699</v>
+      </c>
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="46">
+        <v>5.8136830574803199E-2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="46">
+        <v>0.122011510602144</v>
+      </c>
+      <c r="I4" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4">
+        <v>0.33871948325068701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="46">
+        <v>8.0681967192910403E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="46">
+        <v>0.20922568993037699</v>
+      </c>
+      <c r="E5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="46">
+        <v>5.7806279129921902E-2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="46">
+        <v>0.12186753637424901</v>
+      </c>
+      <c r="I5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5">
+        <v>0.33678601578749601</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="46">
+        <v>8.0652305189098203E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="46">
+        <v>0.207890380542192</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6" s="46">
+        <v>5.77349779197514E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="46">
+        <v>0.119782042435402</v>
+      </c>
+      <c r="I6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6">
+        <v>0.31564108520770501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="46">
+        <v>8.0512376305084496E-2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0.207574905740886</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" s="46">
+        <v>5.7340156734154997E-2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H7" s="46">
+        <v>0.119605093656744</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7">
+        <v>0.29385191616984302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="46">
+        <v>7.9946930876146599E-2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="46">
+        <v>0.207466423164998</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="46">
+        <v>5.7090076900882997E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="46">
+        <v>0.119324063838494</v>
+      </c>
+      <c r="I8" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8">
+        <v>0.29270463095771099</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1">
+      <c r="A9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1">
+      <c r="A10" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="46">
+        <v>5.1875094440202697E-2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="46">
+        <v>0.108855627286852</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="46">
+        <v>5.18797425295573E-2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H11" s="46">
+        <v>0.11343263127560101</v>
+      </c>
+      <c r="I11" t="s">
+        <v>83</v>
+      </c>
+      <c r="J11">
+        <v>0.100695667547159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="46">
+        <v>4.9598120396631397E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="46">
+        <v>0.10732098816654401</v>
+      </c>
+      <c r="E12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="46">
+        <v>5.1779267779870297E-2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="46">
+        <v>0.110466190947479</v>
+      </c>
+      <c r="I12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12">
+        <v>0.100688103601433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="46">
+        <v>4.7910981807108198E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="46">
+        <v>0.104904586048196</v>
+      </c>
+      <c r="E13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="46">
+        <v>5.16262896561639E-2</v>
+      </c>
+      <c r="G13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="46">
+        <v>0.10530737670354599</v>
+      </c>
+      <c r="I13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13">
+        <v>9.9628700240668097E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="46">
+        <v>4.6075918109879897E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="46">
+        <v>0.10485555945991799</v>
+      </c>
+      <c r="E14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="46">
+        <v>5.1039266690062597E-2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" s="46">
+        <v>8.4860784537279493E-2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14">
+        <v>9.9373137204768994E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="46">
+        <v>4.2149207120850102E-2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="46">
+        <v>0.102375500876286</v>
+      </c>
+      <c r="E15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="46">
+        <v>5.0943410611189899E-2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" s="46">
+        <v>8.3439072441641796E-2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15">
+        <v>9.7570645820662202E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="str">
+        <f>RIGHT(A4,8)</f>
+        <v>0.065_1</v>
+      </c>
+      <c r="C17" t="str">
+        <f>RIGHT(C4,9)</f>
+        <v>0.06_0.5</v>
+      </c>
+      <c r="E17" t="str">
+        <f>RIGHT(E11,9)</f>
+        <v>0.095_1.5</v>
+      </c>
+      <c r="G17" t="str">
+        <f>RIGHT(G4,9)</f>
+        <v>0.075_1.5</v>
+      </c>
+      <c r="I17" t="str">
+        <f>RIGHT(I4,8)</f>
+        <v>0_0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="str">
+        <f t="shared" ref="A18:C21" si="0">RIGHT(A5,8)</f>
+        <v>0_0.04_1</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" ref="C18:E21" si="1">RIGHT(C5,9)</f>
+        <v>0.065_0.5</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" ref="E17:G21" si="2">RIGHT(E12,9)</f>
+        <v>0.1_1.5</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" ref="G18:I18" si="3">RIGHT(G5,9)</f>
+        <v>.075_1.25</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" ref="I18:I21" si="4">RIGHT(I5,8)</f>
+        <v>0_0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>0_0.03_1</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>0.095_0.5</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>0.09_1.5</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" ref="G19:I19" si="5">RIGHT(G6,9)</f>
+        <v>0.085_1.5</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="4"/>
+        <v>0_1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>0.045_1</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v>0.1_0.5</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>.095_1.25</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" ref="G20:I20" si="6">RIGHT(G7,9)</f>
+        <v>.085_1.25</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="4"/>
+        <v>0.09_0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>0.035_1</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>0.075_0.5</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>0.1_1.25</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" ref="G21:I21" si="7">RIGHT(G8,9)</f>
+        <v>0.08_1.5</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="4"/>
+        <v>.095_0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A2:J2"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>